<commit_message>
Some Work on Local Variance and Spectral Clustering
</commit_message>
<xml_diff>
--- a/Local Variance/Results/Local_Variance_1.xlsx
+++ b/Local Variance/Results/Local_Variance_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiang\OneDrive\Desktop\Math 199\Spectral Clustering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiang\OneDrive\Desktop\Math 199\Local Variance\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" activeCellId="8" sqref="A3 E5 A4 A6 E3 A8 E7 A10 E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,18 +436,18 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>207302</v>
       </c>
       <c r="B3">
         <v>47.53924266881144</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>206300</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>207301</v>
       </c>
       <c r="B4">
@@ -457,12 +464,12 @@
       <c r="B5">
         <v>47.101783429578468</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>207301</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>206300</v>
       </c>
       <c r="B6">
@@ -479,12 +486,12 @@
       <c r="B7">
         <v>33.793693977544336</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>208903</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>208904</v>
       </c>
       <c r="B8">
@@ -506,13 +513,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>208801</v>
       </c>
       <c r="B10">
         <v>30.451302428121217</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>208801</v>
       </c>
     </row>
@@ -1124,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" activeCellId="8" sqref="A3 E5 A4 A5 E9 A6 E3 A10 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,18 +1162,18 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>207302</v>
       </c>
       <c r="B3">
         <v>61.472899092651851</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>206300</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>207301</v>
       </c>
       <c r="B4">
@@ -1177,18 +1184,18 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>206200</v>
       </c>
       <c r="B5">
         <v>61.135224965465923</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>207301</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>206300</v>
       </c>
       <c r="B6">
@@ -1205,7 +1212,7 @@
       <c r="B7">
         <v>51.593616122370207</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>208903</v>
       </c>
     </row>
@@ -1227,12 +1234,12 @@
       <c r="B9">
         <v>32.943298206169942</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>206200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>208904</v>
       </c>
       <c r="B10">

</xml_diff>